<commit_message>
Resultados WSCAD2021 Special Issue
</commit_message>
<xml_diff>
--- a/sniper/tools/results_cpu2006.xlsx
+++ b/sniper/tools/results_cpu2006.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>Execution Time</t>
   </si>
@@ -34,7 +34,13 @@
     <t>Donuts-50</t>
   </si>
   <si>
+    <t>Donuts-63</t>
+  </si>
+  <si>
     <t>Donuts-75</t>
+  </si>
+  <si>
+    <t>Donuts-88</t>
   </si>
   <si>
     <t>Donuts-100</t>
@@ -431,41 +437,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:26">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="M1" s="1"/>
-      <c r="N1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
+      <c r="Q1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:26">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -477,649 +493,1039 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="O2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="T2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="Y2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:26">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>258059468</v>
       </c>
       <c r="C4">
+        <v>260896868</v>
+      </c>
+      <c r="D4">
         <v>259255068</v>
       </c>
-      <c r="D4">
+      <c r="E4">
+        <v>259731468</v>
+      </c>
+      <c r="F4">
         <v>260687868</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>15635395</v>
       </c>
-      <c r="F4">
+      <c r="H4">
+        <v>15648333</v>
+      </c>
+      <c r="I4">
         <v>15641027</v>
       </c>
-      <c r="G4">
+      <c r="J4">
+        <v>15634345</v>
+      </c>
+      <c r="K4">
         <v>15639351</v>
       </c>
-      <c r="H4">
+      <c r="L4">
         <v>7797345</v>
       </c>
-      <c r="I4">
+      <c r="M4">
+        <v>7810232</v>
+      </c>
+      <c r="N4">
         <v>7802365</v>
       </c>
-      <c r="J4">
+      <c r="O4">
+        <v>7795811</v>
+      </c>
+      <c r="P4">
         <v>7800294</v>
       </c>
-      <c r="K4">
+      <c r="Q4">
         <v>0.6</v>
       </c>
-      <c r="L4">
+      <c r="R4">
         <v>0.6</v>
       </c>
-      <c r="M4">
+      <c r="S4">
         <v>0.6</v>
       </c>
-      <c r="N4">
+      <c r="T4">
+        <v>0.6</v>
+      </c>
+      <c r="U4">
+        <v>0.6</v>
+      </c>
+      <c r="V4">
         <v>489</v>
       </c>
-      <c r="O4">
+      <c r="W4">
+        <v>390</v>
+      </c>
+      <c r="X4">
         <v>326</v>
       </c>
-      <c r="P4">
+      <c r="Y4">
+        <v>278</v>
+      </c>
+      <c r="Z4">
         <v>244</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:26">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>1333713405</v>
       </c>
       <c r="C5">
+        <v>1337840605</v>
+      </c>
+      <c r="D5">
         <v>1330682205</v>
       </c>
-      <c r="D5">
+      <c r="E5">
+        <v>1332682605</v>
+      </c>
+      <c r="F5">
         <v>1400816805</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>42727363</v>
       </c>
-      <c r="F5">
+      <c r="H5">
+        <v>42732455</v>
+      </c>
+      <c r="I5">
         <v>42710139</v>
       </c>
-      <c r="G5">
+      <c r="J5">
+        <v>42710152</v>
+      </c>
+      <c r="K5">
         <v>42985719</v>
       </c>
-      <c r="H5">
+      <c r="L5">
         <v>17665738</v>
       </c>
-      <c r="I5">
+      <c r="M5">
+        <v>17667413</v>
+      </c>
+      <c r="N5">
         <v>17658613</v>
       </c>
-      <c r="J5">
+      <c r="O5">
+        <v>17657219</v>
+      </c>
+      <c r="P5">
         <v>17632008</v>
       </c>
-      <c r="K5">
+      <c r="Q5">
         <v>0.32</v>
       </c>
-      <c r="L5">
+      <c r="R5">
+        <v>0.31</v>
+      </c>
+      <c r="S5">
         <v>0.32</v>
       </c>
-      <c r="M5">
+      <c r="T5">
+        <v>0.32</v>
+      </c>
+      <c r="U5">
         <v>0.3</v>
       </c>
-      <c r="N5">
+      <c r="V5">
         <v>1863</v>
       </c>
-      <c r="O5">
+      <c r="W5">
+        <v>1377</v>
+      </c>
+      <c r="X5">
         <v>1011</v>
       </c>
-      <c r="P5">
+      <c r="Y5">
+        <v>798</v>
+      </c>
+      <c r="Z5">
         <v>662</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:26">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>1260515250</v>
       </c>
       <c r="C6">
+        <v>1255398250</v>
+      </c>
+      <c r="D6">
         <v>1264726450</v>
       </c>
-      <c r="D6">
+      <c r="E6">
+        <v>1255329650</v>
+      </c>
+      <c r="F6">
         <v>1046639850</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>40962039</v>
       </c>
-      <c r="F6">
+      <c r="H6">
+        <v>40861252</v>
+      </c>
+      <c r="I6">
         <v>40843968</v>
       </c>
-      <c r="G6">
+      <c r="J6">
+        <v>40880393</v>
+      </c>
+      <c r="K6">
         <v>40676399</v>
       </c>
-      <c r="H6">
+      <c r="L6">
         <v>17239429</v>
       </c>
-      <c r="I6">
+      <c r="M6">
+        <v>17147663</v>
+      </c>
+      <c r="N6">
         <v>17138148</v>
       </c>
-      <c r="J6">
+      <c r="O6">
+        <v>17123093</v>
+      </c>
+      <c r="P6">
         <v>16923844</v>
       </c>
-      <c r="K6">
+      <c r="Q6">
         <v>0.32</v>
       </c>
-      <c r="L6">
+      <c r="R6">
         <v>0.32</v>
       </c>
-      <c r="M6">
+      <c r="S6">
+        <v>0.32</v>
+      </c>
+      <c r="T6">
+        <v>0.32</v>
+      </c>
+      <c r="U6">
         <v>0.38</v>
       </c>
-      <c r="N6">
+      <c r="V6">
         <v>29429</v>
       </c>
-      <c r="O6">
+      <c r="W6">
+        <v>24211</v>
+      </c>
+      <c r="X6">
         <v>19639</v>
       </c>
-      <c r="P6">
+      <c r="Y6">
+        <v>16540</v>
+      </c>
+      <c r="Z6">
         <v>1427</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:26">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>2075815268</v>
       </c>
       <c r="C7">
+        <v>2064489868</v>
+      </c>
+      <c r="D7">
         <v>2067025068</v>
       </c>
-      <c r="D7">
+      <c r="E7">
+        <v>2064905868</v>
+      </c>
+      <c r="F7">
         <v>2069848268</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>59521121</v>
       </c>
-      <c r="F7">
+      <c r="H7">
+        <v>59231672</v>
+      </c>
+      <c r="I7">
         <v>59059256</v>
       </c>
-      <c r="G7">
+      <c r="J7">
+        <v>58830565</v>
+      </c>
+      <c r="K7">
         <v>58767019</v>
       </c>
-      <c r="H7">
+      <c r="L7">
         <v>25846712</v>
       </c>
-      <c r="I7">
+      <c r="M7">
+        <v>25557271</v>
+      </c>
+      <c r="N7">
         <v>25384859</v>
       </c>
-      <c r="J7">
+      <c r="O7">
+        <v>25156049</v>
+      </c>
+      <c r="P7">
         <v>25086111</v>
       </c>
-      <c r="K7">
+      <c r="Q7">
         <v>0.28</v>
       </c>
-      <c r="L7">
+      <c r="R7">
         <v>0.28</v>
       </c>
-      <c r="M7">
+      <c r="S7">
         <v>0.28</v>
       </c>
-      <c r="N7">
+      <c r="T7">
+        <v>0.28</v>
+      </c>
+      <c r="U7">
+        <v>0.28</v>
+      </c>
+      <c r="V7">
         <v>2160</v>
       </c>
-      <c r="O7">
+      <c r="W7">
+        <v>1685</v>
+      </c>
+      <c r="X7">
         <v>1401</v>
       </c>
-      <c r="P7">
+      <c r="Y7">
+        <v>1063</v>
+      </c>
+      <c r="Z7">
         <v>937</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:26">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>379124658</v>
       </c>
       <c r="C8">
+        <v>389019258</v>
+      </c>
+      <c r="D8">
         <v>393308658</v>
       </c>
-      <c r="D8">
+      <c r="E8">
+        <v>401715458</v>
+      </c>
+      <c r="F8">
         <v>399890658</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>10035385</v>
       </c>
-      <c r="F8">
+      <c r="H8">
+        <v>10012884</v>
+      </c>
+      <c r="I8">
         <v>9996766</v>
       </c>
-      <c r="G8">
+      <c r="J8">
+        <v>9982014</v>
+      </c>
+      <c r="K8">
         <v>9962705</v>
       </c>
-      <c r="H8">
+      <c r="L8">
         <v>4971506</v>
       </c>
-      <c r="I8">
+      <c r="M8">
+        <v>4954166</v>
+      </c>
+      <c r="N8">
         <v>4939801</v>
       </c>
-      <c r="J8">
+      <c r="O8">
+        <v>4925319</v>
+      </c>
+      <c r="P8">
         <v>4905245</v>
       </c>
-      <c r="K8">
+      <c r="Q8">
         <v>0.26</v>
       </c>
-      <c r="L8">
+      <c r="R8">
         <v>0.25</v>
       </c>
-      <c r="M8">
+      <c r="S8">
+        <v>0.25</v>
+      </c>
+      <c r="T8">
         <v>0.24</v>
       </c>
-      <c r="N8">
+      <c r="U8">
+        <v>0.24</v>
+      </c>
+      <c r="V8">
         <v>426</v>
       </c>
-      <c r="O8">
+      <c r="W8">
+        <v>318</v>
+      </c>
+      <c r="X8">
         <v>253</v>
       </c>
-      <c r="P8">
+      <c r="Y8">
+        <v>209</v>
+      </c>
+      <c r="Z8">
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:26">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>2103519875</v>
       </c>
       <c r="C9">
+        <v>2098049875</v>
+      </c>
+      <c r="D9">
         <v>2087914075</v>
       </c>
-      <c r="D9">
+      <c r="E9">
+        <v>2091481875</v>
+      </c>
+      <c r="F9">
         <v>1943766875</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>54099775</v>
       </c>
-      <c r="F9">
+      <c r="H9">
+        <v>53963045</v>
+      </c>
+      <c r="I9">
         <v>53842792</v>
       </c>
-      <c r="G9">
+      <c r="J9">
+        <v>53453166</v>
+      </c>
+      <c r="K9">
         <v>53227554</v>
       </c>
-      <c r="H9">
+      <c r="L9">
         <v>15198900</v>
       </c>
-      <c r="I9">
+      <c r="M9">
+        <v>15125506</v>
+      </c>
+      <c r="N9">
         <v>15096344</v>
       </c>
-      <c r="J9">
+      <c r="O9">
+        <v>14921931</v>
+      </c>
+      <c r="P9">
         <v>14748312</v>
       </c>
-      <c r="K9">
+      <c r="Q9">
         <v>0.25</v>
       </c>
-      <c r="L9">
+      <c r="R9">
         <v>0.25</v>
       </c>
-      <c r="M9">
+      <c r="S9">
+        <v>0.25</v>
+      </c>
+      <c r="T9">
+        <v>0.25</v>
+      </c>
+      <c r="U9">
         <v>0.27</v>
       </c>
-      <c r="N9">
+      <c r="V9">
         <v>1492</v>
       </c>
-      <c r="O9">
+      <c r="W9">
+        <v>1063</v>
+      </c>
+      <c r="X9">
         <v>859</v>
       </c>
-      <c r="P9">
+      <c r="Y9">
+        <v>685</v>
+      </c>
+      <c r="Z9">
         <v>570</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:26">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>798969668</v>
       </c>
       <c r="C10">
+        <v>799815668</v>
+      </c>
+      <c r="D10">
         <v>798296468</v>
       </c>
-      <c r="D10">
+      <c r="E10">
+        <v>798344468</v>
+      </c>
+      <c r="F10">
         <v>799452268</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>16878906</v>
       </c>
-      <c r="F10">
+      <c r="H10">
+        <v>16862278</v>
+      </c>
+      <c r="I10">
         <v>16855075</v>
       </c>
-      <c r="G10">
+      <c r="J10">
+        <v>16848979</v>
+      </c>
+      <c r="K10">
         <v>16844291</v>
       </c>
-      <c r="H10">
+      <c r="L10">
         <v>8448980</v>
       </c>
-      <c r="I10">
+      <c r="M10">
+        <v>8432445</v>
+      </c>
+      <c r="N10">
         <v>8425586</v>
       </c>
-      <c r="J10">
+      <c r="O10">
+        <v>8419699</v>
+      </c>
+      <c r="P10">
         <v>8414806</v>
       </c>
-      <c r="K10">
+      <c r="Q10">
         <v>0.21</v>
       </c>
-      <c r="L10">
+      <c r="R10">
         <v>0.21</v>
       </c>
-      <c r="M10">
+      <c r="S10">
         <v>0.21</v>
       </c>
-      <c r="N10">
+      <c r="T10">
+        <v>0.21</v>
+      </c>
+      <c r="U10">
+        <v>0.21</v>
+      </c>
+      <c r="V10">
         <v>586</v>
       </c>
-      <c r="O10">
+      <c r="W10">
+        <v>453</v>
+      </c>
+      <c r="X10">
         <v>369</v>
       </c>
-      <c r="P10">
+      <c r="Y10">
+        <v>312</v>
+      </c>
+      <c r="Z10">
         <v>272</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:26">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>774127688</v>
       </c>
       <c r="C11">
+        <v>770425488</v>
+      </c>
+      <c r="D11">
         <v>767602688</v>
       </c>
-      <c r="D11">
+      <c r="E11">
+        <v>767184888</v>
+      </c>
+      <c r="F11">
         <v>768038888</v>
       </c>
-      <c r="E11">
+      <c r="G11">
         <v>16721635</v>
       </c>
-      <c r="F11">
+      <c r="H11">
+        <v>16475753</v>
+      </c>
+      <c r="I11">
         <v>16196522</v>
       </c>
-      <c r="G11">
+      <c r="J11">
+        <v>15972285</v>
+      </c>
+      <c r="K11">
         <v>15683513</v>
       </c>
-      <c r="H11">
+      <c r="L11">
         <v>7061838</v>
       </c>
-      <c r="I11">
+      <c r="M11">
+        <v>6836615</v>
+      </c>
+      <c r="N11">
         <v>6579163</v>
       </c>
-      <c r="J11">
+      <c r="O11">
+        <v>6357307</v>
+      </c>
+      <c r="P11">
         <v>6050721</v>
       </c>
-      <c r="K11">
+      <c r="Q11">
         <v>0.21</v>
       </c>
-      <c r="L11">
+      <c r="R11">
         <v>0.21</v>
       </c>
-      <c r="M11">
+      <c r="S11">
+        <v>0.21</v>
+      </c>
+      <c r="T11">
         <v>0.2</v>
       </c>
-      <c r="N11">
+      <c r="U11">
+        <v>0.2</v>
+      </c>
+      <c r="V11">
         <v>1700</v>
       </c>
-      <c r="O11">
+      <c r="W11">
+        <v>1235</v>
+      </c>
+      <c r="X11">
         <v>949</v>
       </c>
-      <c r="P11">
+      <c r="Y11">
+        <v>775</v>
+      </c>
+      <c r="Z11">
         <v>636</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:26">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>2394284668</v>
       </c>
       <c r="C12">
+        <v>2403994268</v>
+      </c>
+      <c r="D12">
         <v>2386809068</v>
       </c>
-      <c r="D12">
+      <c r="E12">
+        <v>2387739868</v>
+      </c>
+      <c r="F12">
         <v>2363983868</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>44349646</v>
       </c>
-      <c r="F12">
+      <c r="H12">
+        <v>44359504</v>
+      </c>
+      <c r="I12">
         <v>44274293</v>
       </c>
-      <c r="G12">
+      <c r="J12">
+        <v>44198404</v>
+      </c>
+      <c r="K12">
         <v>43987143</v>
       </c>
-      <c r="H12">
+      <c r="L12">
         <v>9151443</v>
       </c>
-      <c r="I12">
+      <c r="M12">
+        <v>9076991</v>
+      </c>
+      <c r="N12">
         <v>9025979</v>
       </c>
-      <c r="J12">
+      <c r="O12">
+        <v>8991838</v>
+      </c>
+      <c r="P12">
         <v>8920671</v>
       </c>
-      <c r="K12">
+      <c r="Q12">
         <v>0.18</v>
       </c>
-      <c r="L12">
+      <c r="R12">
         <v>0.18</v>
       </c>
-      <c r="M12">
+      <c r="S12">
         <v>0.18</v>
       </c>
-      <c r="N12">
+      <c r="T12">
+        <v>0.18</v>
+      </c>
+      <c r="U12">
+        <v>0.18</v>
+      </c>
+      <c r="V12">
         <v>2142</v>
       </c>
-      <c r="O12">
+      <c r="W12">
+        <v>1322</v>
+      </c>
+      <c r="X12">
         <v>948</v>
       </c>
-      <c r="P12">
+      <c r="Y12">
+        <v>731</v>
+      </c>
+      <c r="Z12">
         <v>553</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:26">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>1781454782</v>
       </c>
       <c r="C13">
+        <v>1775056182</v>
+      </c>
+      <c r="D13">
         <v>1786020982</v>
       </c>
-      <c r="D13">
+      <c r="E13">
+        <v>1773203982</v>
+      </c>
+      <c r="F13">
         <v>1773781182</v>
       </c>
-      <c r="E13">
+      <c r="G13">
         <v>32028162</v>
       </c>
-      <c r="F13">
+      <c r="H13">
+        <v>32025212</v>
+      </c>
+      <c r="I13">
         <v>32084794</v>
       </c>
-      <c r="G13">
+      <c r="J13">
+        <v>32186322</v>
+      </c>
+      <c r="K13">
         <v>32214808</v>
       </c>
-      <c r="H13">
+      <c r="L13">
         <v>9532948</v>
       </c>
-      <c r="I13">
+      <c r="M13">
+        <v>9519300</v>
+      </c>
+      <c r="N13">
         <v>9516743</v>
       </c>
-      <c r="J13">
+      <c r="O13">
+        <v>9506862</v>
+      </c>
+      <c r="P13">
         <v>9503473</v>
       </c>
-      <c r="K13">
+      <c r="Q13">
         <v>0.17</v>
       </c>
-      <c r="L13">
+      <c r="R13">
+        <v>0.18</v>
+      </c>
+      <c r="S13">
         <v>0.17</v>
       </c>
-      <c r="M13">
+      <c r="T13">
         <v>0.18</v>
       </c>
-      <c r="N13">
+      <c r="U13">
+        <v>0.18</v>
+      </c>
+      <c r="V13">
         <v>851</v>
       </c>
-      <c r="O13">
+      <c r="W13">
+        <v>673</v>
+      </c>
+      <c r="X13">
         <v>522</v>
       </c>
-      <c r="P13">
+      <c r="Y13">
+        <v>423</v>
+      </c>
+      <c r="Z13">
         <v>368</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:26">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>1776679688</v>
       </c>
       <c r="C14">
+        <v>1774796888</v>
+      </c>
+      <c r="D14">
         <v>1775867688</v>
       </c>
-      <c r="D14">
+      <c r="E14">
+        <v>1776137888</v>
+      </c>
+      <c r="F14">
         <v>1764545688</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>19342456</v>
       </c>
-      <c r="F14">
+      <c r="H14">
+        <v>19341753</v>
+      </c>
+      <c r="I14">
         <v>19336343</v>
       </c>
-      <c r="G14">
+      <c r="J14">
+        <v>19340323</v>
+      </c>
+      <c r="K14">
         <v>19347489</v>
       </c>
-      <c r="H14">
+      <c r="L14">
         <v>3676226</v>
       </c>
-      <c r="I14">
+      <c r="M14">
+        <v>3674672</v>
+      </c>
+      <c r="N14">
         <v>3670038</v>
       </c>
-      <c r="J14">
+      <c r="O14">
+        <v>3674095</v>
+      </c>
+      <c r="P14">
         <v>3680940</v>
       </c>
-      <c r="K14">
+      <c r="Q14">
         <v>0.1</v>
       </c>
-      <c r="L14">
+      <c r="R14">
         <v>0.1</v>
       </c>
-      <c r="M14">
+      <c r="S14">
         <v>0.1</v>
       </c>
-      <c r="N14">
+      <c r="T14">
+        <v>0.1</v>
+      </c>
+      <c r="U14">
+        <v>0.1</v>
+      </c>
+      <c r="V14">
         <v>1186</v>
       </c>
-      <c r="O14">
+      <c r="W14">
+        <v>920</v>
+      </c>
+      <c r="X14">
         <v>713</v>
       </c>
-      <c r="P14">
+      <c r="Y14">
+        <v>640</v>
+      </c>
+      <c r="Z14">
         <v>534</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:26">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B15">
         <v>519415670</v>
       </c>
       <c r="C15">
+        <v>519497270</v>
+      </c>
+      <c r="D15">
         <v>518656870</v>
       </c>
-      <c r="D15">
+      <c r="E15">
+        <v>518358270</v>
+      </c>
+      <c r="F15">
         <v>518261470</v>
       </c>
-      <c r="E15">
+      <c r="G15">
         <v>3544129</v>
       </c>
-      <c r="F15">
+      <c r="H15">
+        <v>3521531</v>
+      </c>
+      <c r="I15">
         <v>3502809</v>
       </c>
-      <c r="G15">
+      <c r="J15">
+        <v>3505421</v>
+      </c>
+      <c r="K15">
         <v>3490373</v>
       </c>
-      <c r="H15">
+      <c r="L15">
         <v>1704816</v>
       </c>
-      <c r="I15">
+      <c r="M15">
+        <v>1682136</v>
+      </c>
+      <c r="N15">
         <v>1663363</v>
       </c>
-      <c r="J15">
+      <c r="O15">
+        <v>1664450</v>
+      </c>
+      <c r="P15">
         <v>1649968</v>
       </c>
-      <c r="K15">
+      <c r="Q15">
         <v>0.06</v>
       </c>
-      <c r="L15">
+      <c r="R15">
         <v>0.06</v>
       </c>
-      <c r="M15">
+      <c r="S15">
         <v>0.06</v>
       </c>
-      <c r="N15">
+      <c r="T15">
+        <v>0.06</v>
+      </c>
+      <c r="U15">
+        <v>0.06</v>
+      </c>
+      <c r="V15">
         <v>219</v>
       </c>
-      <c r="O15">
+      <c r="W15">
+        <v>150</v>
+      </c>
+      <c r="X15">
         <v>114</v>
       </c>
-      <c r="P15">
+      <c r="Y15">
+        <v>93</v>
+      </c>
+      <c r="Z15">
         <v>79</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="V1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Início da implementação de diferentes políticas de commit de blocos sujos da cache
</commit_message>
<xml_diff>
--- a/sniper/tools/results_cpu2006.xlsx
+++ b/sniper/tools/results_cpu2006.xlsx
@@ -14,12 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="19">
+  <si>
+    <t>Runtime</t>
+  </si>
+  <si>
+    <t>Average Bandwidth Usage</t>
+  </si>
   <si>
     <t>Memory Access</t>
   </si>
   <si>
-    <t>Runtime</t>
+    <t>Memory Writes</t>
+  </si>
+  <si>
+    <t>Memory Logs</t>
+  </si>
+  <si>
+    <t>Memory Buffer Overflow</t>
+  </si>
+  <si>
+    <t>Number of Checkpoints</t>
   </si>
   <si>
     <t>donuts-wb1</t>
@@ -413,13 +428,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:BL5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:64">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -443,191 +458,656 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
+      <c r="T1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AV1" s="1"/>
+      <c r="AW1" s="1"/>
+      <c r="AX1" s="1"/>
+      <c r="AY1" s="1"/>
+      <c r="AZ1" s="1"/>
+      <c r="BA1" s="1"/>
+      <c r="BB1" s="1"/>
+      <c r="BC1" s="1"/>
+      <c r="BD1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="BE1" s="1"/>
+      <c r="BF1" s="1"/>
+      <c r="BG1" s="1"/>
+      <c r="BH1" s="1"/>
+      <c r="BI1" s="1"/>
+      <c r="BJ1" s="1"/>
+      <c r="BK1" s="1"/>
+      <c r="BL1" s="1"/>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:64">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="X2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AY2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="BC2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="BD2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BE2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="BF2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BH2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="BI2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BK2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="BL2" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:64">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:64">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B4">
+        <v>259877668</v>
+      </c>
+      <c r="C4">
+        <v>260275868</v>
+      </c>
+      <c r="D4">
+        <v>260326068</v>
+      </c>
+      <c r="E4">
+        <v>260239068</v>
+      </c>
+      <c r="F4">
+        <v>260089468</v>
+      </c>
+      <c r="G4">
+        <v>259716868</v>
+      </c>
+      <c r="H4">
+        <v>260080068</v>
+      </c>
+      <c r="I4">
+        <v>260046068</v>
+      </c>
+      <c r="J4">
+        <v>259957068</v>
+      </c>
+      <c r="K4">
+        <v>0.6</v>
+      </c>
+      <c r="L4">
+        <v>0.6</v>
+      </c>
+      <c r="M4">
+        <v>0.6</v>
+      </c>
+      <c r="N4">
+        <v>0.6</v>
+      </c>
+      <c r="O4">
+        <v>0.6</v>
+      </c>
+      <c r="P4">
+        <v>0.6</v>
+      </c>
+      <c r="Q4">
+        <v>0.6</v>
+      </c>
+      <c r="R4">
+        <v>0.6</v>
+      </c>
+      <c r="S4">
+        <v>0.6</v>
+      </c>
+      <c r="T4">
         <v>15631340</v>
       </c>
-      <c r="C4">
+      <c r="U4">
         <v>15631798</v>
       </c>
-      <c r="D4">
+      <c r="V4">
         <v>15634752</v>
       </c>
-      <c r="E4">
+      <c r="W4">
         <v>15651273</v>
       </c>
-      <c r="F4">
+      <c r="X4">
         <v>15632790</v>
       </c>
-      <c r="G4">
+      <c r="Y4">
         <v>15631618</v>
       </c>
-      <c r="H4">
+      <c r="Z4">
         <v>15632185</v>
       </c>
-      <c r="I4">
+      <c r="AA4">
         <v>15632182</v>
       </c>
-      <c r="J4">
+      <c r="AB4">
         <v>15633168</v>
       </c>
-      <c r="K4">
-        <v>259877668</v>
-      </c>
-      <c r="L4">
-        <v>260275868</v>
-      </c>
-      <c r="M4">
-        <v>260326068</v>
-      </c>
-      <c r="N4">
-        <v>260239068</v>
-      </c>
-      <c r="O4">
-        <v>260089468</v>
-      </c>
-      <c r="P4">
-        <v>259716868</v>
-      </c>
-      <c r="Q4">
-        <v>260080068</v>
-      </c>
-      <c r="R4">
-        <v>260046068</v>
-      </c>
-      <c r="S4">
-        <v>259957068</v>
+      <c r="AC4">
+        <v>7791945</v>
+      </c>
+      <c r="AD4">
+        <v>7791480</v>
+      </c>
+      <c r="AE4">
+        <v>7794262</v>
+      </c>
+      <c r="AF4">
+        <v>7811028</v>
+      </c>
+      <c r="AG4">
+        <v>7792477</v>
+      </c>
+      <c r="AH4">
+        <v>7791849</v>
+      </c>
+      <c r="AI4">
+        <v>7791793</v>
+      </c>
+      <c r="AJ4">
+        <v>7791835</v>
+      </c>
+      <c r="AK4">
+        <v>7792666</v>
+      </c>
+      <c r="AL4">
+        <v>7839395</v>
+      </c>
+      <c r="AM4">
+        <v>7840318</v>
+      </c>
+      <c r="AN4">
+        <v>7840490</v>
+      </c>
+      <c r="AO4">
+        <v>7840245</v>
+      </c>
+      <c r="AP4">
+        <v>7840313</v>
+      </c>
+      <c r="AQ4">
+        <v>7839769</v>
+      </c>
+      <c r="AR4">
+        <v>7840392</v>
+      </c>
+      <c r="AS4">
+        <v>7840347</v>
+      </c>
+      <c r="AT4">
+        <v>7840502</v>
+      </c>
+      <c r="AU4">
+        <v>122490</v>
+      </c>
+      <c r="AV4">
+        <v>122504</v>
+      </c>
+      <c r="AW4">
+        <v>122507</v>
+      </c>
+      <c r="AX4">
+        <v>122503</v>
+      </c>
+      <c r="AY4">
+        <v>122504</v>
+      </c>
+      <c r="AZ4">
+        <v>122496</v>
+      </c>
+      <c r="BA4">
+        <v>122506</v>
+      </c>
+      <c r="BB4">
+        <v>122505</v>
+      </c>
+      <c r="BC4">
+        <v>122507</v>
+      </c>
+      <c r="BD4">
+        <v>320</v>
+      </c>
+      <c r="BE4">
+        <v>320</v>
+      </c>
+      <c r="BF4">
+        <v>320</v>
+      </c>
+      <c r="BG4">
+        <v>321</v>
+      </c>
+      <c r="BH4">
+        <v>320</v>
+      </c>
+      <c r="BI4">
+        <v>320</v>
+      </c>
+      <c r="BJ4">
+        <v>320</v>
+      </c>
+      <c r="BK4">
+        <v>320</v>
+      </c>
+      <c r="BL4">
+        <v>320</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:64">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B5">
+        <v>2408330068</v>
+      </c>
+      <c r="C5">
+        <v>2403930268</v>
+      </c>
+      <c r="D5">
+        <v>2394831468</v>
+      </c>
+      <c r="E5">
+        <v>2367314468</v>
+      </c>
+      <c r="F5">
+        <v>2364194068</v>
+      </c>
+      <c r="G5">
+        <v>2362812268</v>
+      </c>
+      <c r="H5">
+        <v>2370611268</v>
+      </c>
+      <c r="I5">
+        <v>2389238868</v>
+      </c>
+      <c r="J5">
+        <v>2405323268</v>
+      </c>
+      <c r="K5">
+        <v>0.18</v>
+      </c>
+      <c r="L5">
+        <v>0.18</v>
+      </c>
+      <c r="M5">
+        <v>0.18</v>
+      </c>
+      <c r="N5">
+        <v>0.18</v>
+      </c>
+      <c r="O5">
+        <v>0.18</v>
+      </c>
+      <c r="P5">
+        <v>0.18</v>
+      </c>
+      <c r="Q5">
+        <v>0.18</v>
+      </c>
+      <c r="R5">
+        <v>0.18</v>
+      </c>
+      <c r="S5">
+        <v>0.18</v>
+      </c>
+      <c r="T5">
         <v>44130115</v>
       </c>
-      <c r="C5">
+      <c r="U5">
         <v>44115820</v>
       </c>
-      <c r="D5">
+      <c r="V5">
         <v>43990937</v>
       </c>
-      <c r="E5">
+      <c r="W5">
         <v>43990570</v>
       </c>
-      <c r="F5">
+      <c r="X5">
         <v>43988394</v>
       </c>
-      <c r="G5">
+      <c r="Y5">
         <v>43979666</v>
       </c>
-      <c r="H5">
+      <c r="Z5">
         <v>43972867</v>
       </c>
-      <c r="I5">
+      <c r="AA5">
         <v>43966633</v>
       </c>
-      <c r="J5">
+      <c r="AB5">
         <v>44125734</v>
       </c>
-      <c r="K5">
-        <v>2408330068</v>
-      </c>
-      <c r="L5">
-        <v>2403930268</v>
-      </c>
-      <c r="M5">
-        <v>2394831468</v>
-      </c>
-      <c r="N5">
-        <v>2367314468</v>
-      </c>
-      <c r="O5">
-        <v>2364194068</v>
-      </c>
-      <c r="P5">
-        <v>2362812268</v>
-      </c>
-      <c r="Q5">
-        <v>2370611268</v>
-      </c>
-      <c r="R5">
-        <v>2389238868</v>
-      </c>
-      <c r="S5">
-        <v>2405323268</v>
+      <c r="AC5">
+        <v>8958203</v>
+      </c>
+      <c r="AD5">
+        <v>8970527</v>
+      </c>
+      <c r="AE5">
+        <v>8935016</v>
+      </c>
+      <c r="AF5">
+        <v>8922952</v>
+      </c>
+      <c r="AG5">
+        <v>8924999</v>
+      </c>
+      <c r="AH5">
+        <v>8927577</v>
+      </c>
+      <c r="AI5">
+        <v>8924407</v>
+      </c>
+      <c r="AJ5">
+        <v>8930759</v>
+      </c>
+      <c r="AK5">
+        <v>8968247</v>
+      </c>
+      <c r="AL5">
+        <v>35171912</v>
+      </c>
+      <c r="AM5">
+        <v>35145293</v>
+      </c>
+      <c r="AN5">
+        <v>35055921</v>
+      </c>
+      <c r="AO5">
+        <v>35067618</v>
+      </c>
+      <c r="AP5">
+        <v>35063395</v>
+      </c>
+      <c r="AQ5">
+        <v>35052089</v>
+      </c>
+      <c r="AR5">
+        <v>35048460</v>
+      </c>
+      <c r="AS5">
+        <v>35035874</v>
+      </c>
+      <c r="AT5">
+        <v>35157487</v>
+      </c>
+      <c r="AU5">
+        <v>549561</v>
+      </c>
+      <c r="AV5">
+        <v>549145</v>
+      </c>
+      <c r="AW5">
+        <v>547748</v>
+      </c>
+      <c r="AX5">
+        <v>547931</v>
+      </c>
+      <c r="AY5">
+        <v>547865</v>
+      </c>
+      <c r="AZ5">
+        <v>547688</v>
+      </c>
+      <c r="BA5">
+        <v>547632</v>
+      </c>
+      <c r="BB5">
+        <v>547435</v>
+      </c>
+      <c r="BC5">
+        <v>549335</v>
+      </c>
+      <c r="BD5">
+        <v>556</v>
+      </c>
+      <c r="BE5">
+        <v>562</v>
+      </c>
+      <c r="BF5">
+        <v>566</v>
+      </c>
+      <c r="BG5">
+        <v>558</v>
+      </c>
+      <c r="BH5">
+        <v>558</v>
+      </c>
+      <c r="BI5">
+        <v>559</v>
+      </c>
+      <c r="BJ5">
+        <v>558</v>
+      </c>
+      <c r="BK5">
+        <v>560</v>
+      </c>
+      <c r="BL5">
+        <v>562</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="7">
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="K1:S1"/>
+    <mergeCell ref="T1:AB1"/>
+    <mergeCell ref="AC1:AK1"/>
+    <mergeCell ref="AL1:AT1"/>
+    <mergeCell ref="AU1:BC1"/>
+    <mergeCell ref="BD1:BL1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>